<commit_message>
update strike data and logs; add new CWL inputs and remove outdated entries
</commit_message>
<xml_diff>
--- a/inputs/war_bases.xlsx
+++ b/inputs/war_bases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>#</t>
   </si>
@@ -46,106 +46,94 @@
     <t>Satan</t>
   </si>
   <si>
+    <t>fwa</t>
+  </si>
+  <si>
     <t>BumblinMumbler</t>
   </si>
   <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>Smitty™</t>
+  </si>
+  <si>
     <t>Sned</t>
   </si>
   <si>
-    <t>Smitty™</t>
-  </si>
-  <si>
-    <t>pg</t>
-  </si>
-  <si>
     <t>pi314ever</t>
   </si>
   <si>
+    <t>Vojt</t>
+  </si>
+  <si>
+    <t>hype</t>
+  </si>
+  <si>
+    <t>Ascended</t>
+  </si>
+  <si>
+    <t>Anas</t>
+  </si>
+  <si>
+    <t>ImagineWaggons</t>
+  </si>
+  <si>
     <t>Protips</t>
   </si>
   <si>
-    <t>Big Daddy T</t>
-  </si>
-  <si>
-    <t>Vojt</t>
-  </si>
-  <si>
-    <t>Anas</t>
-  </si>
-  <si>
-    <t>ImagineWaggons</t>
-  </si>
-  <si>
-    <t>hype</t>
-  </si>
-  <si>
-    <t>Ascended</t>
+    <t>Marlec</t>
+  </si>
+  <si>
+    <t>K.L.A.U.S</t>
   </si>
   <si>
     <t>Rod</t>
   </si>
   <si>
-    <t>Marlec</t>
+    <t>Welli</t>
   </si>
   <si>
     <t>Mythos</t>
   </si>
   <si>
-    <t>Welli</t>
+    <t>sanskar</t>
   </si>
   <si>
     <t>Sham</t>
   </si>
   <si>
-    <t>3STAR Warrior</t>
-  </si>
-  <si>
-    <t>sanskar</t>
-  </si>
-  <si>
-    <t>fwa</t>
+    <t>LOGAN911</t>
+  </si>
+  <si>
+    <t>Dalto</t>
+  </si>
+  <si>
+    <t>ERDNUSSFLIP</t>
+  </si>
+  <si>
+    <t>NagaStoleMyBike</t>
+  </si>
+  <si>
+    <t>Carsonn</t>
   </si>
   <si>
     <t>Motz</t>
   </si>
   <si>
-    <t>Dalto</t>
-  </si>
-  <si>
-    <t>ERDNUSSFLIP</t>
-  </si>
-  <si>
-    <t>NagaStoleMyBike</t>
-  </si>
-  <si>
     <t>DNG</t>
   </si>
   <si>
     <t>CrazyWaveIT</t>
   </si>
   <si>
+    <t>Truthful Lies</t>
+  </si>
+  <si>
     <t>Limit?</t>
   </si>
   <si>
-    <t>appable</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>SirFluffyy</t>
-  </si>
-  <si>
-    <t>LOGAN911</t>
-  </si>
-  <si>
-    <t>Truthful Lies</t>
-  </si>
-  <si>
-    <t>Az7777</t>
-  </si>
-  <si>
-    <t>W1nter</t>
   </si>
   <si>
     <t>RoyalOne</t>
@@ -475,10 +463,12 @@
         <v>10</v>
       </c>
       <c r="C2" s="4">
-        <f t="shared" ref="C2:C36" si="2">COUNTA(D2:J2)</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="5"/>
+        <f t="shared" ref="C2:C32" si="2">COUNTA(D2:J2)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -492,7 +482,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4">
         <f t="shared" si="2"/>
@@ -505,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="2"/>
@@ -518,7 +508,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="2"/>
@@ -531,7 +521,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="2"/>
@@ -544,7 +534,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="2"/>
@@ -557,7 +547,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="2"/>
@@ -570,7 +560,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="2"/>
@@ -583,7 +573,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="2"/>
@@ -596,7 +586,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="2"/>
@@ -609,7 +599,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="2"/>
@@ -622,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="2"/>
@@ -642,11 +632,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15">
@@ -655,7 +648,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="2"/>
@@ -668,7 +661,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="2"/>
@@ -681,11 +674,32 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18">
@@ -694,7 +708,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="2"/>
@@ -707,7 +721,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="2"/>
@@ -727,7 +741,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="2"/>
@@ -740,17 +754,11 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -802,13 +810,7 @@
       </c>
       <c r="C25" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -851,7 +853,7 @@
     </row>
     <row r="29">
       <c r="A29" s="3">
-        <f t="shared" ref="A29:A36" si="3">row()-1</f>
+        <f t="shared" ref="A29:A32" si="3">row()-1</f>
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -872,7 +874,28 @@
       </c>
       <c r="C30" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31">
@@ -885,7 +908,16 @@
       </c>
       <c r="C31" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="32">
@@ -898,68 +930,6 @@
       </c>
       <c r="C32" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="3">
-        <f t="shared" si="3"/>
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="3">
-        <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="3">
-        <f t="shared" si="3"/>
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="4">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>